<commit_message>
Commit changes required to create test files for next step: creating new file structure
</commit_message>
<xml_diff>
--- a/Record Keeping/Seeds Already Tested.xlsx
+++ b/Record Keeping/Seeds Already Tested.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="-40" windowWidth="11440" windowHeight="14220" tabRatio="500"/>
+    <workbookView xWindow="15340" yWindow="-720" windowWidth="11440" windowHeight="14220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,32 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Seed</t>
   </si>
   <si>
-    <t>Pharmacy Tech Programs</t>
-  </si>
-  <si>
-    <t>Pharmacy Technician Certification</t>
-  </si>
-  <si>
-    <t>Pharmacy Technician Programs</t>
-  </si>
-  <si>
-    <t>Pharmacy Technician School</t>
-  </si>
-  <si>
-    <t>Pharmacy Technician Training</t>
-  </si>
-  <si>
-    <t>Physical Therapy Programs</t>
-  </si>
-  <si>
-    <t>Physical Therapy Schools</t>
-  </si>
-  <si>
     <t>Psychology Degree</t>
   </si>
   <si>
@@ -69,24 +48,6 @@
     <t>Real Estate Schools</t>
   </si>
   <si>
-    <t>Restaurant Management Degree</t>
-  </si>
-  <si>
-    <t>Security Classes</t>
-  </si>
-  <si>
-    <t>Security Guard College</t>
-  </si>
-  <si>
-    <t>Security Guard Training</t>
-  </si>
-  <si>
-    <t>Security Officer Training</t>
-  </si>
-  <si>
-    <t>Security Training</t>
-  </si>
-  <si>
     <t>Social Work Degree</t>
   </si>
   <si>
@@ -168,15 +129,6 @@
     <t>CNA Training</t>
   </si>
   <si>
-    <t>Criminal Justice Degree</t>
-  </si>
-  <si>
-    <t>CSI College</t>
-  </si>
-  <si>
-    <t>CSI School</t>
-  </si>
-  <si>
     <t>EMT Certification</t>
   </si>
   <si>
@@ -192,57 +144,6 @@
     <t>EMT School</t>
   </si>
   <si>
-    <t>Fashion College</t>
-  </si>
-  <si>
-    <t>Fashion Courses</t>
-  </si>
-  <si>
-    <t>Fashion Design Classes</t>
-  </si>
-  <si>
-    <t>Fashion Design Courses</t>
-  </si>
-  <si>
-    <t>Fashion Design Schools</t>
-  </si>
-  <si>
-    <t>Fashion Merchandising Schools</t>
-  </si>
-  <si>
-    <t>Fashion Schools</t>
-  </si>
-  <si>
-    <t>Fire School</t>
-  </si>
-  <si>
-    <t>Firefighter Training</t>
-  </si>
-  <si>
-    <t>Event Planning Certification</t>
-  </si>
-  <si>
-    <t>Event Planning Classes</t>
-  </si>
-  <si>
-    <t>Event Planning Courses</t>
-  </si>
-  <si>
-    <t>Event Planning Schools</t>
-  </si>
-  <si>
-    <t>Hospitality Degree</t>
-  </si>
-  <si>
-    <t>Hospitality Management Degree</t>
-  </si>
-  <si>
-    <t>Hospitality Schools</t>
-  </si>
-  <si>
-    <t>Hotel Management Degree</t>
-  </si>
-  <si>
     <t>HR Certification</t>
   </si>
   <si>
@@ -252,18 +153,6 @@
     <t>Human Resources Certification</t>
   </si>
   <si>
-    <t>IT Classes</t>
-  </si>
-  <si>
-    <t>IT Courses</t>
-  </si>
-  <si>
-    <t>IT Schools</t>
-  </si>
-  <si>
-    <t>IT Training</t>
-  </si>
-  <si>
     <t>LPN Classes</t>
   </si>
   <si>
@@ -273,15 +162,6 @@
     <t>LPN Training</t>
   </si>
   <si>
-    <t>Marketing Classes</t>
-  </si>
-  <si>
-    <t>Marketing Courses</t>
-  </si>
-  <si>
-    <t>Marketing Degree</t>
-  </si>
-  <si>
     <t>Personal Trainer Certification</t>
   </si>
   <si>
@@ -292,9 +172,6 @@
   </si>
   <si>
     <t>Acupuncture Schools</t>
-  </si>
-  <si>
-    <t>Fashion Colleges</t>
   </si>
   <si>
     <t>Massage Therapy Schools</t>
@@ -358,8 +235,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -370,13 +269,35 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -706,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A97"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:XFD76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -721,482 +642,277 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>